<commit_message>
Starting redesign of opening page. SS
</commit_message>
<xml_diff>
--- a/new marketing page plus sessions.xlsx
+++ b/new marketing page plus sessions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15100" windowHeight="10230"/>
+    <workbookView xWindow="1650" yWindow="0" windowWidth="15100" windowHeight="10230"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -475,12 +475,12 @@
   <dimension ref="A2:A39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="65.7265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="94.26953125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:1" ht="18.5" x14ac:dyDescent="0.45">

</xml_diff>